<commit_message>
JD Unternehmen -> Veranstaltung & Kategorie geloescht
</commit_message>
<xml_diff>
--- a/eingabe/Schuelerwuensche.xlsx
+++ b/eingabe/Schuelerwuensche.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\+++Schule\LF12\Projekt Berufsorientierungstag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekt\eingabe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D3104B-4063-45C2-8F55-2225ED32774C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA82443D-C1E4-4D93-9D30-D78ADBA78438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wahl" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="278">
   <si>
     <t>Klasse</t>
   </si>
@@ -857,9 +857,6 @@
   </si>
   <si>
     <t>Tahir</t>
-  </si>
-  <si>
-    <t>Unternehmen</t>
   </si>
 </sst>
 </file>
@@ -1717,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9D0705-4684-4B32-B343-DBA4607380EC}">
-  <dimension ref="A1:M136"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M28"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1726,7 @@
     <col min="9" max="9" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,11 +1754,8 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1771,33 +1765,8 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>18</v>
-      </c>
-      <c r="F2">
-        <v>19</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>14</v>
-      </c>
-      <c r="I2">
-        <v>22</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <f>COUNTIF(Wahlbereich,L2)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1816,24 +1785,8 @@
       <c r="F3">
         <v>9</v>
       </c>
-      <c r="G3">
-        <v>18</v>
-      </c>
-      <c r="H3">
-        <v>19</v>
-      </c>
-      <c r="I3">
-        <v>15</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <f>COUNTIF(Wahlbereich,L3)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1846,30 +1799,8 @@
       <c r="D4">
         <v>20</v>
       </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>15</v>
-      </c>
-      <c r="H4">
-        <v>26</v>
-      </c>
-      <c r="I4">
-        <v>11</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-      <c r="M4">
-        <f>COUNTIF(Wahlbereich,L4)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1897,15 +1828,8 @@
       <c r="I5">
         <v>15</v>
       </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="M5">
-        <f>COUNTIF(Wahlbereich,L5)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1933,15 +1857,8 @@
       <c r="I6">
         <v>23</v>
       </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-      <c r="M6">
-        <f>COUNTIF(Wahlbereich,L6)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1969,15 +1886,8 @@
       <c r="I7">
         <v>23</v>
       </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-      <c r="M7">
-        <f>COUNTIF(Wahlbereich,L7)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2005,15 +1915,8 @@
       <c r="I8">
         <v>25</v>
       </c>
-      <c r="L8">
-        <v>7</v>
-      </c>
-      <c r="M8">
-        <f>COUNTIF(Wahlbereich,L8)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2041,15 +1944,8 @@
       <c r="I9">
         <v>26</v>
       </c>
-      <c r="L9">
-        <v>8</v>
-      </c>
-      <c r="M9">
-        <f>COUNTIF(Wahlbereich,L9)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2077,15 +1973,8 @@
       <c r="I10">
         <v>22</v>
       </c>
-      <c r="L10">
-        <v>9</v>
-      </c>
-      <c r="M10">
-        <f>COUNTIF(Wahlbereich,L10)</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2113,15 +2002,8 @@
       <c r="I11">
         <v>16</v>
       </c>
-      <c r="L11">
-        <v>10</v>
-      </c>
-      <c r="M11">
-        <f>COUNTIF(Wahlbereich,L11)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2149,15 +2031,8 @@
       <c r="I12">
         <v>9</v>
       </c>
-      <c r="L12">
-        <v>11</v>
-      </c>
-      <c r="M12">
-        <f>COUNTIF(Wahlbereich,L12)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2185,15 +2060,8 @@
       <c r="I13">
         <v>22</v>
       </c>
-      <c r="L13">
-        <v>12</v>
-      </c>
-      <c r="M13">
-        <f>COUNTIF(Wahlbereich,L13)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2221,15 +2089,8 @@
       <c r="I14">
         <v>16</v>
       </c>
-      <c r="L14">
-        <v>13</v>
-      </c>
-      <c r="M14">
-        <f>COUNTIF(Wahlbereich,L14)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2257,15 +2118,8 @@
       <c r="I15">
         <v>26</v>
       </c>
-      <c r="L15">
-        <v>14</v>
-      </c>
-      <c r="M15">
-        <f>COUNTIF(Wahlbereich,L15)</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2293,15 +2147,8 @@
       <c r="I16">
         <v>18</v>
       </c>
-      <c r="L16">
-        <v>15</v>
-      </c>
-      <c r="M16">
-        <f>COUNTIF(Wahlbereich,L16)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2329,15 +2176,8 @@
       <c r="I17">
         <v>10</v>
       </c>
-      <c r="L17">
-        <v>16</v>
-      </c>
-      <c r="M17">
-        <f>COUNTIF(Wahlbereich,L17)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2365,15 +2205,8 @@
       <c r="I18">
         <v>11</v>
       </c>
-      <c r="L18">
-        <v>17</v>
-      </c>
-      <c r="M18">
-        <f>COUNTIF(Wahlbereich,L18)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2401,15 +2234,8 @@
       <c r="I19">
         <v>6</v>
       </c>
-      <c r="L19">
-        <v>18</v>
-      </c>
-      <c r="M19">
-        <f>COUNTIF(Wahlbereich,L19)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2437,15 +2263,8 @@
       <c r="I20">
         <v>13</v>
       </c>
-      <c r="L20">
-        <v>19</v>
-      </c>
-      <c r="M20">
-        <f>COUNTIF(Wahlbereich,L20)</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2473,15 +2292,8 @@
       <c r="I21">
         <v>19</v>
       </c>
-      <c r="L21">
-        <v>20</v>
-      </c>
-      <c r="M21">
-        <f>COUNTIF(Wahlbereich,L21)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -2509,15 +2321,8 @@
       <c r="I22">
         <v>25</v>
       </c>
-      <c r="L22">
-        <v>21</v>
-      </c>
-      <c r="M22">
-        <f>COUNTIF(Wahlbereich,L22)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2545,15 +2350,8 @@
       <c r="I23">
         <v>16</v>
       </c>
-      <c r="L23">
-        <v>22</v>
-      </c>
-      <c r="M23">
-        <f>COUNTIF(Wahlbereich,L23)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2581,15 +2379,8 @@
       <c r="I24">
         <v>19</v>
       </c>
-      <c r="L24">
-        <v>23</v>
-      </c>
-      <c r="M24">
-        <f>COUNTIF(Wahlbereich,L24)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -2617,15 +2408,8 @@
       <c r="I25">
         <v>9</v>
       </c>
-      <c r="L25">
-        <v>24</v>
-      </c>
-      <c r="M25">
-        <f>COUNTIF(Wahlbereich,L25)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2653,15 +2437,8 @@
       <c r="I26">
         <v>11</v>
       </c>
-      <c r="L26">
-        <v>25</v>
-      </c>
-      <c r="M26">
-        <f>COUNTIF(Wahlbereich,L26)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2689,15 +2466,8 @@
       <c r="I27">
         <v>1</v>
       </c>
-      <c r="L27">
-        <v>26</v>
-      </c>
-      <c r="M27">
-        <f>COUNTIF(Wahlbereich,L27)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -2725,15 +2495,8 @@
       <c r="I28">
         <v>13</v>
       </c>
-      <c r="L28">
-        <v>27</v>
-      </c>
-      <c r="M28">
-        <f>COUNTIF(Wahlbereich,L28)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2762,7 +2525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2791,7 +2554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2820,7 +2583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>

</xml_diff>